<commit_message>
Changed test file to Strings
</commit_message>
<xml_diff>
--- a/testData.xlsx
+++ b/testData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Max\sortCompare\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60E7E141-CEA2-4E63-B684-CB3F4B2468D9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53133B05-BFAB-4F93-BBAC-4F572FF43F21}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{52E7C980-E13A-41BB-A47F-B2931F872586}"/>
   </bookViews>
@@ -30,7 +30,41 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>sad</t>
+  </si>
+  <si>
+    <t>doggy</t>
+  </si>
+  <si>
+    <t>fight</t>
+  </si>
+  <si>
+    <t>josh</t>
+  </si>
+  <si>
+    <t>orange</t>
+  </si>
+  <si>
+    <t>wario</t>
+  </si>
+  <si>
+    <t>cool</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -380,10 +414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79B0D28F-9DEE-4590-AA67-223E389B27AA}">
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -392,37 +426,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2">
         <v>12</v>
       </c>
-      <c r="B1">
+      <c r="B2">
         <v>4000</v>
       </c>
-      <c r="C1">
+      <c r="C2">
         <v>230</v>
       </c>
-      <c r="D1">
+      <c r="D2">
         <v>15</v>
       </c>
-      <c r="E1">
+      <c r="E2">
         <v>1</v>
       </c>
-      <c r="F1">
+      <c r="F2">
         <v>-1</v>
       </c>
-      <c r="G1">
+      <c r="G2">
         <v>-1234</v>
       </c>
-      <c r="H1">
+      <c r="H2">
         <v>234324</v>
       </c>
-      <c r="I1">
+      <c r="I2">
         <v>2</v>
       </c>
-      <c r="J1">
+      <c r="J2">
         <v>34234</v>
       </c>
-      <c r="K1">
+      <c r="K2">
         <v>100000000</v>
       </c>
     </row>

</xml_diff>